<commit_message>
Refactor ImportAlokasi action to use firstOrNew for creating records and update confirmation text in SusenasAlokasi resource
</commit_message>
<xml_diff>
--- a/storage/app/public/templates/m5hNJw8cEbEEIcW5Rofo0qwhBoUXGFPgehc2o3Sx.xlsx
+++ b/storage/app/public/templates/m5hNJw8cEbEEIcW5Rofo0qwhBoUXGFPgehc2o3Sx.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11003"/>
-  <workbookPr defaultThemeVersion="202300"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29530"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/muhlis/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ACER\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0C7FF2CF-0D83-6841-8BE2-1AC2A1ED4DE9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F13E146B-B505-4B02-853D-259F3492A994}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20480" yWindow="500" windowWidth="20480" windowHeight="22540" xr2:uid="{2BB00275-CFEA-CC42-9DB3-DC1754C04F33}"/>
+    <workbookView xWindow="135" yWindow="780" windowWidth="28665" windowHeight="14385" xr2:uid="{2BB00275-CFEA-CC42-9DB3-DC1754C04F33}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,23 +20,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="16">
   <si>
     <t>Kode PCL</t>
   </si>
@@ -81,6 +70,9 @@
   </si>
   <si>
     <t>151126</t>
+  </si>
+  <si>
+    <t>Jumlah Sampel</t>
   </si>
 </sst>
 </file>
@@ -453,21 +445,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{47605DD0-9331-5A4D-A50F-48DAA8F4C3CE}">
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="4" width="10.83203125" style="1"/>
-    <col min="5" max="5" width="31.1640625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="10.83203125" style="1"/>
-    <col min="7" max="7" width="24.83203125" style="1" customWidth="1"/>
+    <col min="1" max="4" width="10.875" style="1"/>
+    <col min="5" max="5" width="31.125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="10.875" style="1"/>
+    <col min="7" max="7" width="24.875" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>4</v>
       </c>
@@ -489,8 +481,11 @@
       <c r="G1" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="H1" s="1" t="s">
+        <v>15</v>
+      </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>7</v>
       </c>
@@ -512,8 +507,11 @@
       <c r="G2" s="1" t="s">
         <v>13</v>
       </c>
+      <c r="H2">
+        <v>10</v>
+      </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>7</v>
       </c>
@@ -534,6 +532,9 @@
       </c>
       <c r="G3" s="1" t="s">
         <v>13</v>
+      </c>
+      <c r="H3">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>